<commit_message>
finished delete section and course
</commit_message>
<xml_diff>
--- a/World_Countries_second+cities.xlsx
+++ b/World_Countries_second+cities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigbry\Projects\source\repos\SQL\Bluelime\Building_SQL_With_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1CE2F5-146D-4E36-B598-4BCE0807C801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF728A35-E341-4B33-8FB0-051E831DCF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1215" yWindow="-120" windowWidth="22905" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="238">
   <si>
     <t>country</t>
   </si>
@@ -744,7 +744,10 @@
     <t>Comma</t>
   </si>
   <si>
-    <t>SQL_Query</t>
+    <t>SQL_Query_Update_New_Value</t>
+  </si>
+  <si>
+    <t>SQL_Query_Delete_Value</t>
   </si>
 </sst>
 </file>
@@ -892,24 +895,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1023,6 +1008,24 @@
       <font>
         <b/>
         <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -1060,12 +1063,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D34E46A-82FE-41CF-BF3F-59E781B51DF2}" name="Table2" displayName="Table2" ref="A1:K198" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="5">
-  <autoFilter ref="A1:K198" xr:uid="{5D34E46A-82FE-41CF-BF3F-59E781B51DF2}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CCE1A096-CDDE-4583-9780-1E11586B2BC2}" name="Country_Id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{78181417-AF46-4599-8CEB-48A74F69B430}" name="country" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{946096CF-962C-4EFF-BAFD-AF3DF165EFF6}" name="second city" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D34E46A-82FE-41CF-BF3F-59E781B51DF2}" name="Table2" displayName="Table2" ref="A1:L198" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:L198" xr:uid="{5D34E46A-82FE-41CF-BF3F-59E781B51DF2}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{CCE1A096-CDDE-4583-9780-1E11586B2BC2}" name="Country_Id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{78181417-AF46-4599-8CEB-48A74F69B430}" name="country" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{946096CF-962C-4EFF-BAFD-AF3DF165EFF6}" name="second city" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{499E8870-F137-4BFB-8B50-77589569AAC3}" name="Query_1"/>
     <tableColumn id="5" xr3:uid="{B3D16AB0-703E-48DA-A5D9-BBE51294F419}" name="Query_2">
       <calculatedColumnFormula>A2</calculatedColumnFormula>
@@ -1085,8 +1088,11 @@
     <tableColumn id="10" xr3:uid="{394E7376-0C1D-4653-AFAC-BA9D0E11D454}" name="Comma">
       <calculatedColumnFormula>CHAR(44)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{96FE7DFF-441A-478F-820E-9F6564848EC9}" name="SQL_Query" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{96FE7DFF-441A-478F-820E-9F6564848EC9}" name="SQL_Query_Update_New_Value" dataDxfId="0">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{90189E57-F78A-48ED-B2EF-8A90E81E38FA}" name="SQL_Query_Delete_Value">
+      <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1414,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K203"/>
+  <dimension ref="A1:L203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L2:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,9 +1438,10 @@
     <col min="8" max="9" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" customWidth="1"/>
     <col min="11" max="11" width="133.42578125" customWidth="1"/>
+    <col min="12" max="12" width="104.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>227</v>
       </c>
@@ -1468,8 +1475,11 @@
       <c r="K1" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1510,8 +1520,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Kandahar' WHERE [dbo].[Countries].[Country_ID] = 1;</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 1;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1552,8 +1566,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Berat' WHERE [dbo].[Countries].[Country_ID] = 2;</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 2;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1594,8 +1612,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Oran' WHERE [dbo].[Countries].[Country_ID] = 3;</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 3;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1636,8 +1658,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Encamp' WHERE [dbo].[Countries].[Country_ID] = 4;</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 4;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1678,8 +1704,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Bungo' WHERE [dbo].[Countries].[Country_ID] = 5;</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 5;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1720,8 +1750,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='All Saints' WHERE [dbo].[Countries].[Country_ID] = 6;</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 6;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1762,8 +1796,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='La Plata' WHERE [dbo].[Countries].[Country_ID] = 7;</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 7;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1804,8 +1842,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Sevan' WHERE [dbo].[Countries].[Country_ID] = 8;</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 8;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1846,8 +1888,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Tasmania' WHERE [dbo].[Countries].[Country_ID] = 9;</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 9;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1888,8 +1934,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Graz' WHERE [dbo].[Countries].[Country_ID] = 10;</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 10;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1930,8 +1980,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Astara' WHERE [dbo].[Countries].[Country_ID] = 11;</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 11;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1972,8 +2026,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Clarence Town' WHERE [dbo].[Countries].[Country_ID] = 12;</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 12;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2014,8 +2072,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Mahooz' WHERE [dbo].[Countries].[Country_ID] = 13;</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 13;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -2056,8 +2118,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Khulna' WHERE [dbo].[Countries].[Country_ID] = 14;</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 14;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2098,8 +2164,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Saint Michael' WHERE [dbo].[Countries].[Country_ID] = 15;</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 15;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -2140,8 +2210,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Orsha' WHERE [dbo].[Countries].[Country_ID] = 16;</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 16;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2182,8 +2256,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Antwerp' WHERE [dbo].[Countries].[Country_ID] = 17;</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 17;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -2224,8 +2302,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Dangriga' WHERE [dbo].[Countries].[Country_ID] = 18;</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 18;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2266,8 +2348,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Kandi' WHERE [dbo].[Countries].[Country_ID] = 19;</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 19;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -2308,8 +2394,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Mongar' WHERE [dbo].[Countries].[Country_ID] = 20;</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 20;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2350,8 +2440,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Montero' WHERE [dbo].[Countries].[Country_ID] = 21;</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 21;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -2392,8 +2486,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Jajce' WHERE [dbo].[Countries].[Country_ID] = 22;</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 22;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2434,8 +2532,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Kanye' WHERE [dbo].[Countries].[Country_ID] = 23;</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 23;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2476,8 +2578,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Sao Paulo' WHERE [dbo].[Countries].[Country_ID] = 24;</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 24;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2518,8 +2624,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Sukang' WHERE [dbo].[Countries].[Country_ID] = 25;</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 25;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -2560,8 +2670,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Pleven' WHERE [dbo].[Countries].[Country_ID] = 26;</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 26;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2602,8 +2716,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Boromo' WHERE [dbo].[Countries].[Country_ID] = 27;</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 27;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -2644,8 +2762,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='Ngozi' WHERE [dbo].[Countries].[Country_ID] = 28;</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 28;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2684,8 +2806,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 29;</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 29;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2724,8 +2850,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 30;</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 30;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2764,8 +2894,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 31;</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 31;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>32</v>
       </c>
@@ -2804,8 +2938,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 32;</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 32;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2844,8 +2982,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 33;</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 33;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>34</v>
       </c>
@@ -2884,8 +3026,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 34;</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 34;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2924,8 +3070,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 35;</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 35;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>36</v>
       </c>
@@ -2964,8 +3114,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 36;</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 36;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -3004,8 +3158,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 37;</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 37;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>38</v>
       </c>
@@ -3044,8 +3202,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 38;</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 38;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -3084,8 +3246,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 39;</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 39;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -3124,8 +3290,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 40;</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 40;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -3164,8 +3334,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 41;</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 41;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -3204,8 +3378,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 42;</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 42;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -3244,8 +3422,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 43;</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 43;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>44</v>
       </c>
@@ -3284,8 +3466,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 44;</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 44;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -3324,8 +3510,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 45;</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 45;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>46</v>
       </c>
@@ -3364,8 +3554,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 46;</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 46;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -3404,8 +3598,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 47;</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 47;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -3444,8 +3642,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 48;</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 48;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -3484,8 +3686,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 49;</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 49;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>50</v>
       </c>
@@ -3524,8 +3730,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 50;</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 50;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -3564,8 +3774,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 51;</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 51;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -3604,8 +3818,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 52;</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 52;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -3644,8 +3862,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 53;</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 53;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -3684,8 +3906,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 54;</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 54;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -3724,8 +3950,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 55;</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 55;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>56</v>
       </c>
@@ -3764,8 +3994,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 56;</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 56;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -3804,8 +4038,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 57;</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 57;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>58</v>
       </c>
@@ -3844,8 +4082,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 58;</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 58;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -3884,8 +4126,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 59;</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 59;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>60</v>
       </c>
@@ -3924,8 +4170,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 60;</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 60;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -3964,8 +4214,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 61;</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 61;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>62</v>
       </c>
@@ -4004,8 +4258,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 62;</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 62;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -4044,8 +4302,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 63;</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 63;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -4084,8 +4346,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 64;</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 64;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -4124,8 +4390,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 65;</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 65;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>66</v>
       </c>
@@ -4164,8 +4434,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 66;</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 66;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -4204,8 +4478,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 67;</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 67;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>68</v>
       </c>
@@ -4244,8 +4522,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 68;</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 68;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -4284,8 +4566,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 69;</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 69;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>70</v>
       </c>
@@ -4324,8 +4610,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 70;</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 70;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -4364,8 +4654,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 71;</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 71;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>72</v>
       </c>
@@ -4404,8 +4698,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 72;</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 72;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -4444,8 +4742,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 73;</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 73;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>74</v>
       </c>
@@ -4484,8 +4786,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 74;</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 74;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>75</v>
       </c>
@@ -4524,8 +4830,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 75;</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 75;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>76</v>
       </c>
@@ -4564,8 +4874,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 76;</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 76;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>77</v>
       </c>
@@ -4604,8 +4918,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 77;</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 77;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>78</v>
       </c>
@@ -4644,8 +4962,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 78;</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 78;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -4684,8 +5006,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 79;</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 79;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>80</v>
       </c>
@@ -4724,8 +5050,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 80;</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 80;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>81</v>
       </c>
@@ -4764,8 +5094,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 81;</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 81;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>82</v>
       </c>
@@ -4804,8 +5138,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 82;</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 82;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>83</v>
       </c>
@@ -4844,8 +5182,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 83;</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 83;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>84</v>
       </c>
@@ -4884,8 +5226,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 84;</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 84;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>85</v>
       </c>
@@ -4924,8 +5270,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 85;</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 85;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>86</v>
       </c>
@@ -4964,8 +5314,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 86;</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 86;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>87</v>
       </c>
@@ -5004,8 +5358,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 87;</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 87;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>88</v>
       </c>
@@ -5044,8 +5402,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 88;</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 88;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>89</v>
       </c>
@@ -5084,8 +5446,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 89;</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 89;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>90</v>
       </c>
@@ -5124,8 +5490,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 90;</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 90;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>91</v>
       </c>
@@ -5164,8 +5534,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 91;</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 91;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>92</v>
       </c>
@@ -5204,8 +5578,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 92;</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 92;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>93</v>
       </c>
@@ -5244,8 +5622,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 93;</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 93;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>94</v>
       </c>
@@ -5284,8 +5666,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 94;</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 94;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>95</v>
       </c>
@@ -5324,8 +5710,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 95;</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 95;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>96</v>
       </c>
@@ -5364,8 +5754,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 96;</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 96;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>97</v>
       </c>
@@ -5404,8 +5798,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 97;</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 97;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>98</v>
       </c>
@@ -5444,8 +5842,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 98;</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 98;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>99</v>
       </c>
@@ -5484,8 +5886,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 99;</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L100" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 99;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>100</v>
       </c>
@@ -5524,8 +5930,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 100;</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L101" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 100;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>101</v>
       </c>
@@ -5564,8 +5974,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 101;</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L102" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 101;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>102</v>
       </c>
@@ -5604,8 +6018,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 102;</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L103" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 102;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>103</v>
       </c>
@@ -5644,8 +6062,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 103;</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L104" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 103;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>104</v>
       </c>
@@ -5684,8 +6106,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 104;</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L105" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 104;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>105</v>
       </c>
@@ -5724,8 +6150,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 105;</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L106" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 105;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>106</v>
       </c>
@@ -5764,8 +6194,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 106;</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L107" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 106;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>107</v>
       </c>
@@ -5804,8 +6238,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 107;</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L108" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 107;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>108</v>
       </c>
@@ -5844,8 +6282,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 108;</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L109" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 108;</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>109</v>
       </c>
@@ -5884,8 +6326,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 109;</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L110" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 109;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>110</v>
       </c>
@@ -5924,8 +6370,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 110;</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L111" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 110;</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>111</v>
       </c>
@@ -5964,8 +6414,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 111;</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L112" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 111;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <v>112</v>
       </c>
@@ -6004,8 +6458,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 112;</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L113" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 112;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>113</v>
       </c>
@@ -6044,8 +6502,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 113;</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L114" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 113;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
         <v>114</v>
       </c>
@@ -6084,8 +6546,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 114;</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L115" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 114;</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>115</v>
       </c>
@@ -6124,8 +6590,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 115;</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L116" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 115;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="8">
         <v>116</v>
       </c>
@@ -6164,8 +6634,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 116;</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L117" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 116;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
         <v>117</v>
       </c>
@@ -6204,8 +6678,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 117;</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L118" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 117;</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
         <v>118</v>
       </c>
@@ -6244,8 +6722,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 118;</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L119" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 118;</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>119</v>
       </c>
@@ -6284,8 +6766,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 119;</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L120" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 119;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>120</v>
       </c>
@@ -6324,8 +6810,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 120;</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L121" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 120;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="6">
         <v>121</v>
       </c>
@@ -6364,8 +6854,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 121;</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L122" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 121;</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
         <v>122</v>
       </c>
@@ -6404,8 +6898,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 122;</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L123" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 122;</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="6">
         <v>123</v>
       </c>
@@ -6444,8 +6942,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 123;</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L124" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 123;</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="8">
         <v>124</v>
       </c>
@@ -6484,8 +6986,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 124;</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L125" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 124;</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="6">
         <v>125</v>
       </c>
@@ -6524,8 +7030,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 125;</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L126" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 125;</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
         <v>126</v>
       </c>
@@ -6564,8 +7074,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 126;</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L127" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 126;</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="6">
         <v>127</v>
       </c>
@@ -6604,8 +7118,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 127;</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L128" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 127;</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="8">
         <v>128</v>
       </c>
@@ -6644,8 +7162,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 128;</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L129" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 128;</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="6">
         <v>129</v>
       </c>
@@ -6684,8 +7206,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 129;</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L130" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 129;</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="8">
         <v>130</v>
       </c>
@@ -6724,8 +7250,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 130;</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L131" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 130;</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="6">
         <v>131</v>
       </c>
@@ -6764,8 +7294,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 131;</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L132" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 131;</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="8">
         <v>132</v>
       </c>
@@ -6804,8 +7338,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 132;</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L133" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 132;</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="6">
         <v>133</v>
       </c>
@@ -6844,8 +7382,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 133;</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L134" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 133;</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="8">
         <v>134</v>
       </c>
@@ -6884,8 +7426,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 134;</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L135" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 134;</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="6">
         <v>135</v>
       </c>
@@ -6924,8 +7470,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 135;</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L136" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 135;</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="8">
         <v>136</v>
       </c>
@@ -6964,8 +7514,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 136;</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L137" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 136;</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="6">
         <v>137</v>
       </c>
@@ -7004,8 +7558,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 137;</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L138" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 137;</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="8">
         <v>138</v>
       </c>
@@ -7044,8 +7602,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 138;</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L139" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 138;</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="6">
         <v>139</v>
       </c>
@@ -7084,8 +7646,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 139;</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L140" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 139;</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="8">
         <v>140</v>
       </c>
@@ -7124,8 +7690,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 140;</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L141" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 140;</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="6">
         <v>141</v>
       </c>
@@ -7164,8 +7734,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 141;</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L142" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 141;</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="8">
         <v>142</v>
       </c>
@@ -7204,8 +7778,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 142;</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L143" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 142;</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="6">
         <v>143</v>
       </c>
@@ -7244,8 +7822,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 143;</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L144" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 143;</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="8">
         <v>144</v>
       </c>
@@ -7284,8 +7866,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 144;</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L145" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 144;</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="6">
         <v>145</v>
       </c>
@@ -7324,8 +7910,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 145;</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L146" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 145;</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="8">
         <v>146</v>
       </c>
@@ -7364,8 +7954,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 146;</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L147" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 146;</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="6">
         <v>147</v>
       </c>
@@ -7404,8 +7998,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 147;</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L148" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 147;</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="8">
         <v>148</v>
       </c>
@@ -7444,8 +8042,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 148;</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L149" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 148;</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="6">
         <v>149</v>
       </c>
@@ -7484,8 +8086,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 149;</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L150" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 149;</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="8">
         <v>150</v>
       </c>
@@ -7524,8 +8130,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 150;</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L151" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 150;</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="6">
         <v>151</v>
       </c>
@@ -7564,8 +8174,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 151;</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L152" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 151;</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="8">
         <v>152</v>
       </c>
@@ -7604,8 +8218,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 152;</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L153" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 152;</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>153</v>
       </c>
@@ -7644,8 +8262,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 153;</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L154" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 153;</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="8">
         <v>154</v>
       </c>
@@ -7684,8 +8306,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 154;</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L155" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 154;</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="6">
         <v>155</v>
       </c>
@@ -7724,8 +8350,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 155;</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L156" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 155;</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="8">
         <v>156</v>
       </c>
@@ -7764,8 +8394,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 156;</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L157" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 156;</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="6">
         <v>157</v>
       </c>
@@ -7804,8 +8438,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 157;</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L158" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 157;</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="8">
         <v>158</v>
       </c>
@@ -7844,8 +8482,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 158;</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L159" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 158;</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="6">
         <v>159</v>
       </c>
@@ -7884,8 +8526,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 159;</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L160" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 159;</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="8">
         <v>160</v>
       </c>
@@ -7924,8 +8570,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 160;</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L161" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 160;</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="6">
         <v>161</v>
       </c>
@@ -7964,8 +8614,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 161;</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L162" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 161;</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="8">
         <v>162</v>
       </c>
@@ -8004,8 +8658,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 162;</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L163" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 162;</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="6">
         <v>163</v>
       </c>
@@ -8044,8 +8702,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 163;</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L164" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 163;</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="8">
         <v>164</v>
       </c>
@@ -8084,8 +8746,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 164;</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L165" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 164;</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="6">
         <v>165</v>
       </c>
@@ -8124,8 +8790,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 165;</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L166" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 165;</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="8">
         <v>166</v>
       </c>
@@ -8164,8 +8834,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 166;</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L167" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 166;</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="6">
         <v>167</v>
       </c>
@@ -8204,8 +8878,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 167;</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L168" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 167;</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="8">
         <v>168</v>
       </c>
@@ -8244,8 +8922,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 168;</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L169" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 168;</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="6">
         <v>169</v>
       </c>
@@ -8284,8 +8966,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 169;</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L170" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 169;</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="8">
         <v>170</v>
       </c>
@@ -8324,8 +9010,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 170;</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L171" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 170;</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="6">
         <v>171</v>
       </c>
@@ -8364,8 +9054,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 171;</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L172" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 171;</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="8">
         <v>172</v>
       </c>
@@ -8404,8 +9098,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 172;</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L173" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 172;</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="6">
         <v>173</v>
       </c>
@@ -8444,8 +9142,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 173;</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L174" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 173;</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="8">
         <v>174</v>
       </c>
@@ -8484,8 +9186,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 174;</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L175" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 174;</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="6">
         <v>175</v>
       </c>
@@ -8524,8 +9230,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 175;</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L176" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 175;</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="8">
         <v>176</v>
       </c>
@@ -8564,8 +9274,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 176;</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L177" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 176;</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="6">
         <v>177</v>
       </c>
@@ -8604,8 +9318,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 177;</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L178" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 177;</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="8">
         <v>178</v>
       </c>
@@ -8644,8 +9362,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 178;</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L179" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 178;</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="6">
         <v>179</v>
       </c>
@@ -8684,8 +9406,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 179;</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L180" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 179;</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="8">
         <v>180</v>
       </c>
@@ -8724,8 +9450,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 180;</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L181" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 180;</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="6">
         <v>181</v>
       </c>
@@ -8764,8 +9494,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 181;</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L182" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 181;</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="8">
         <v>182</v>
       </c>
@@ -8804,8 +9538,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 182;</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L183" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 182;</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="6">
         <v>183</v>
       </c>
@@ -8844,8 +9582,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 183;</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L184" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 183;</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="8">
         <v>184</v>
       </c>
@@ -8884,8 +9626,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 184;</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L185" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 184;</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="6">
         <v>185</v>
       </c>
@@ -8924,8 +9670,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 185;</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L186" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 185;</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="8">
         <v>186</v>
       </c>
@@ -8964,8 +9714,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 186;</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L187" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 186;</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="6">
         <v>187</v>
       </c>
@@ -9004,8 +9758,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 187;</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L188" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 187;</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="8">
         <v>188</v>
       </c>
@@ -9044,8 +9802,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 188;</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L189" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 188;</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
         <v>189</v>
       </c>
@@ -9084,8 +9846,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 189;</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L190" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 189;</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="8">
         <v>190</v>
       </c>
@@ -9124,8 +9890,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 190;</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L191" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 190;</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="6">
         <v>191</v>
       </c>
@@ -9164,8 +9934,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 191;</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L192" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 191;</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="8">
         <v>192</v>
       </c>
@@ -9204,8 +9978,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 192;</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L193" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 192;</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="6">
         <v>193</v>
       </c>
@@ -9244,8 +10022,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 193;</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L194" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 193;</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="8">
         <v>194</v>
       </c>
@@ -9284,8 +10066,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 194;</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L195" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 194;</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="6">
         <v>195</v>
       </c>
@@ -9324,8 +10110,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 195;</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L196" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 195;</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="8">
         <v>196</v>
       </c>
@@ -9364,8 +10154,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 196;</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L197" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 196;</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -9404,8 +10198,12 @@
         <f>CONCATENATE(Table2[[#This Row],[Query_1]],Table2[[#This Row],[Quote1]],Table2[[#This Row],[Query_4]],Table2[[#This Row],[Quote1]]," WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
         <v>UPDATE [dbo].[Countries] SET Second_City ='0' WHERE [dbo].[Countries].[Country_ID] = 197;</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L198" t="str">
+        <f>CONCATENATE(Table2[[#This Row],[Query_1]]," NULL WHERE [dbo].[Countries].[Country_ID] = ",Table2[[#This Row],[Query_2]],";")</f>
+        <v>UPDATE [dbo].[Countries] SET Second_City = NULL WHERE [dbo].[Countries].[Country_ID] = 197;</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C203">
         <v>1</v>
       </c>

</xml_diff>